<commit_message>
checkpoint Rapih almost perfect dengan komentar
</commit_message>
<xml_diff>
--- a/Excel/Hasil_Pengujian_Map_128_avg_length.xlsx
+++ b/Excel/Hasil_Pengujian_Map_128_avg_length.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\SEMHAS\TA_Python_Server\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\SEMHAS\TA_Python_Server\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A940303-2048-49D2-ACAD-D4880E2CB0B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E164595-A15D-45E7-B844-F330DAC781A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -611,7 +611,7 @@
   <dimension ref="A1:G65"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J22" sqref="J22"/>
+      <selection activeCell="B2" sqref="B2:F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -645,232 +645,232 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>40</v>
+        <v>7</v>
       </c>
       <c r="C2">
-        <v>2.6330000000000011E-4</v>
+        <v>7.9670000000000001E-4</v>
       </c>
       <c r="D2">
-        <v>8.7900000000000012E-4</v>
+        <v>4.4444999999999997E-3</v>
       </c>
       <c r="E2">
-        <v>2.932300000000001E-3</v>
+        <v>2.9551299999999999E-2</v>
       </c>
       <c r="F2">
-        <v>1.0929700000000001E-2</v>
+        <v>0.19877359999999999</v>
       </c>
       <c r="G2">
-        <v>3.751075E-3</v>
+        <v>5.8391524999999993E-2</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>56</v>
+        <v>8</v>
       </c>
       <c r="C3">
-        <v>3.3599999999999998E-4</v>
+        <v>3.9439999999999988E-4</v>
       </c>
       <c r="D3">
-        <v>9.6270000000000004E-4</v>
+        <v>1.5790000000000001E-3</v>
       </c>
       <c r="E3">
-        <v>2.9889999999999999E-3</v>
+        <v>6.460200000000001E-3</v>
       </c>
       <c r="F3">
-        <v>1.1006200000000001E-2</v>
+        <v>2.7491499999999999E-2</v>
       </c>
       <c r="G3">
-        <v>3.8234749999999998E-3</v>
+        <v>8.9812750000000004E-3</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="B4" t="s">
-        <v>57</v>
+        <v>9</v>
       </c>
       <c r="C4">
-        <v>3.1470000000000001E-4</v>
+        <v>8.7399999999999999E-4</v>
       </c>
       <c r="D4">
-        <v>1.0001999999999999E-3</v>
+        <v>4.3349E-3</v>
       </c>
       <c r="E4">
-        <v>3.0230999999999999E-3</v>
+        <v>2.7797499999999999E-2</v>
       </c>
       <c r="F4">
-        <v>1.1051200000000001E-2</v>
+        <v>0.18007819999999999</v>
       </c>
       <c r="G4">
-        <v>3.8473000000000001E-3</v>
+        <v>5.3271150000000003E-2</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="B5" t="s">
-        <v>66</v>
+        <v>10</v>
       </c>
       <c r="C5">
-        <v>3.8249999999999997E-4</v>
+        <v>8.0180000000000008E-4</v>
       </c>
       <c r="D5">
-        <v>1.0116999999999999E-3</v>
+        <v>4.1804999999999993E-3</v>
       </c>
       <c r="E5">
-        <v>3.2128E-3</v>
+        <v>2.69538E-2</v>
       </c>
       <c r="F5">
-        <v>1.11264E-2</v>
+        <v>0.17773829999999999</v>
       </c>
       <c r="G5">
-        <v>3.9333500000000004E-3</v>
+        <v>5.2418600000000003E-2</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="B6" t="s">
-        <v>60</v>
+        <v>11</v>
       </c>
       <c r="C6">
-        <v>5.2250000000000007E-4</v>
+        <v>5.4959999999999991E-4</v>
       </c>
       <c r="D6">
-        <v>1.5704E-3</v>
+        <v>2.0154999999999999E-3</v>
       </c>
       <c r="E6">
-        <v>3.9540999999999986E-3</v>
+        <v>7.6709999999999999E-3</v>
       </c>
       <c r="F6">
-        <v>1.35342E-2</v>
+        <v>2.8932099999999999E-2</v>
       </c>
       <c r="G6">
-        <v>4.8953E-3</v>
+        <v>9.7920500000000001E-3</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B7" t="s">
-        <v>39</v>
+        <v>12</v>
       </c>
       <c r="C7">
-        <v>4.3110000000000002E-4</v>
+        <v>8.183000000000001E-4</v>
       </c>
       <c r="D7">
-        <v>1.3385000000000001E-3</v>
+        <v>4.5246000000000001E-3</v>
       </c>
       <c r="E7">
-        <v>4.0620000000000014E-3</v>
+        <v>3.0049900000000001E-2</v>
       </c>
       <c r="F7">
-        <v>1.4038999999999999E-2</v>
+        <v>0.20457220000000001</v>
       </c>
       <c r="G7">
-        <v>4.9676500000000014E-3</v>
+        <v>5.9991250000000003E-2</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B8" t="s">
-        <v>44</v>
+        <v>13</v>
       </c>
       <c r="C8">
-        <v>4.6989999999999988E-4</v>
+        <v>8.3429999999999995E-4</v>
       </c>
       <c r="D8">
-        <v>1.4894999999999999E-3</v>
+        <v>4.7235999999999997E-3</v>
       </c>
       <c r="E8">
-        <v>4.9845000000000002E-3</v>
+        <v>3.0702199999999999E-2</v>
       </c>
       <c r="F8">
-        <v>1.31269E-2</v>
+        <v>0.195657</v>
       </c>
       <c r="G8">
-        <v>5.0177000000000008E-3</v>
+        <v>5.7979274999999997E-2</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B9" t="s">
-        <v>54</v>
+        <v>14</v>
       </c>
       <c r="C9">
-        <v>4.8069999999999997E-4</v>
+        <v>5.1900000000000004E-4</v>
       </c>
       <c r="D9">
-        <v>1.3879999999999999E-3</v>
+        <v>2.5062999999999999E-3</v>
       </c>
       <c r="E9">
-        <v>4.1368000000000004E-3</v>
+        <v>1.0818299999999999E-2</v>
       </c>
       <c r="F9">
-        <v>1.4173099999999999E-2</v>
+        <v>5.5259999999999997E-2</v>
       </c>
       <c r="G9">
-        <v>5.0446499999999986E-3</v>
+        <v>1.72759E-2</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B10" t="s">
-        <v>55</v>
+        <v>15</v>
       </c>
       <c r="C10">
-        <v>4.4200000000000001E-4</v>
+        <v>3.5E-4</v>
       </c>
       <c r="D10">
-        <v>1.3045999999999999E-3</v>
+        <v>1.6364999999999999E-3</v>
       </c>
       <c r="E10">
-        <v>3.9623000000000002E-3</v>
+        <v>7.0992E-3</v>
       </c>
       <c r="F10">
-        <v>1.54468E-2</v>
+        <v>3.1927499999999998E-2</v>
       </c>
       <c r="G10">
-        <v>5.2889249999999999E-3</v>
+        <v>1.02533E-2</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="B11" t="s">
-        <v>65</v>
+        <v>16</v>
       </c>
       <c r="C11">
-        <v>4.8720000000000002E-4</v>
+        <v>4.4660000000000001E-4</v>
       </c>
       <c r="D11">
-        <v>1.4147999999999999E-3</v>
+        <v>1.6946000000000001E-3</v>
       </c>
       <c r="E11">
-        <v>4.1064000000000014E-3</v>
+        <v>6.8047999999999997E-3</v>
       </c>
       <c r="F11">
-        <v>1.5676499999999999E-2</v>
+        <v>2.8878500000000001E-2</v>
       </c>
       <c r="G11">
-        <v>5.421225E-3</v>
+        <v>9.4561249999999993E-3</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
@@ -878,91 +878,91 @@
         <v>2</v>
       </c>
       <c r="B12" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="C12">
-        <v>4.7279999999999989E-4</v>
+        <v>4.37E-4</v>
       </c>
       <c r="D12">
-        <v>1.5681E-3</v>
+        <v>1.8249E-3</v>
       </c>
       <c r="E12">
-        <v>4.6663E-3</v>
+        <v>7.0086000000000011E-3</v>
       </c>
       <c r="F12">
-        <v>1.51979E-2</v>
+        <v>2.96522E-2</v>
       </c>
       <c r="G12">
-        <v>5.4762749999999992E-3</v>
+        <v>9.7306750000000011E-3</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B13" t="s">
-        <v>43</v>
+        <v>18</v>
       </c>
       <c r="C13">
-        <v>5.0170000000000011E-4</v>
+        <v>9.1180000000000015E-4</v>
       </c>
       <c r="D13">
-        <v>1.606E-3</v>
+        <v>4.4942999999999997E-3</v>
       </c>
       <c r="E13">
-        <v>4.5802000000000004E-3</v>
+        <v>2.8027300000000002E-2</v>
       </c>
       <c r="F13">
-        <v>1.54742E-2</v>
+        <v>0.17958470000000001</v>
       </c>
       <c r="G13">
-        <v>5.5405250000000001E-3</v>
+        <v>5.3254524999999997E-2</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="B14" t="s">
-        <v>67</v>
+        <v>19</v>
       </c>
       <c r="C14">
-        <v>3.6549999999999999E-4</v>
+        <v>9.9789999999999992E-4</v>
       </c>
       <c r="D14">
-        <v>1.0134E-3</v>
+        <v>4.7220999999999999E-3</v>
       </c>
       <c r="E14">
-        <v>3.6587E-3</v>
+        <v>3.1725499999999997E-2</v>
       </c>
       <c r="F14">
-        <v>1.7533699999999999E-2</v>
+        <v>0.19733619999999999</v>
       </c>
       <c r="G14">
-        <v>5.6428249999999998E-3</v>
+        <v>5.8695425000000009E-2</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="B15" t="s">
-        <v>70</v>
+        <v>20</v>
       </c>
       <c r="C15">
-        <v>3.9350000000000002E-4</v>
+        <v>1.005E-3</v>
       </c>
       <c r="D15">
-        <v>1.0667999999999999E-3</v>
+        <v>5.6778999999999996E-3</v>
       </c>
       <c r="E15">
-        <v>3.7215E-3</v>
+        <v>3.4527299999999997E-2</v>
       </c>
       <c r="F15">
-        <v>1.7754800000000001E-2</v>
+        <v>0.225498</v>
       </c>
       <c r="G15">
-        <v>5.7341500000000004E-3</v>
+        <v>6.6677049999999988E-2</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.3">
@@ -970,229 +970,229 @@
         <v>2</v>
       </c>
       <c r="B16" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C16">
-        <v>4.3209999999999999E-4</v>
+        <v>8.4270000000000005E-4</v>
       </c>
       <c r="D16">
-        <v>1.4465000000000001E-3</v>
+        <v>4.4114000000000002E-3</v>
       </c>
       <c r="E16">
-        <v>4.7888999999999996E-3</v>
+        <v>2.77015E-2</v>
       </c>
       <c r="F16">
-        <v>1.6785999999999999E-2</v>
+        <v>0.17886940000000001</v>
       </c>
       <c r="G16">
-        <v>5.8633750000000014E-3</v>
+        <v>5.2956250000000003E-2</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B17" t="s">
-        <v>62</v>
+        <v>22</v>
       </c>
       <c r="C17">
-        <v>5.1840000000000002E-4</v>
+        <v>8.4049999999999988E-4</v>
       </c>
       <c r="D17">
-        <v>1.6442E-3</v>
+        <v>4.4665E-3</v>
       </c>
       <c r="E17">
-        <v>4.5433000000000001E-3</v>
+        <v>2.62738E-2</v>
       </c>
       <c r="F17">
-        <v>1.68763E-2</v>
+        <v>0.1665604</v>
       </c>
       <c r="G17">
-        <v>5.8955500000000011E-3</v>
+        <v>4.9535299999999997E-2</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A18">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B18" t="s">
-        <v>45</v>
+        <v>23</v>
       </c>
       <c r="C18">
-        <v>4.975E-4</v>
+        <v>4.3209999999999999E-4</v>
       </c>
       <c r="D18">
-        <v>1.5995E-3</v>
+        <v>1.4465000000000001E-3</v>
       </c>
       <c r="E18">
-        <v>4.5439000000000009E-3</v>
+        <v>4.7888999999999996E-3</v>
       </c>
       <c r="F18">
-        <v>1.70324E-2</v>
+        <v>1.6785999999999999E-2</v>
       </c>
       <c r="G18">
-        <v>5.9183250000000012E-3</v>
+        <v>5.8633750000000014E-3</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A19">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B19" t="s">
-        <v>41</v>
+        <v>24</v>
       </c>
       <c r="C19">
-        <v>4.7790000000000002E-4</v>
+        <v>4.7279999999999989E-4</v>
       </c>
       <c r="D19">
-        <v>1.5106E-3</v>
+        <v>1.5681E-3</v>
       </c>
       <c r="E19">
-        <v>4.8173999999999986E-3</v>
+        <v>4.6663E-3</v>
       </c>
       <c r="F19">
-        <v>1.68845E-2</v>
+        <v>1.51979E-2</v>
       </c>
       <c r="G19">
-        <v>5.9226000000000001E-3</v>
+        <v>5.4762749999999992E-3</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A20">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B20" t="s">
-        <v>61</v>
+        <v>25</v>
       </c>
       <c r="C20">
-        <v>5.6980000000000008E-4</v>
+        <v>5.9829999999999996E-4</v>
       </c>
       <c r="D20">
-        <v>1.6581E-3</v>
+        <v>1.7952000000000001E-3</v>
       </c>
       <c r="E20">
-        <v>4.6348000000000014E-3</v>
+        <v>6.3026999999999996E-3</v>
       </c>
       <c r="F20">
-        <v>1.7063499999999999E-2</v>
+        <v>2.30758E-2</v>
       </c>
       <c r="G20">
-        <v>5.9815500000000004E-3</v>
+        <v>7.9430000000000004E-3</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A21">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="B21" t="s">
-        <v>69</v>
+        <v>26</v>
       </c>
       <c r="C21">
-        <v>5.6540000000000008E-4</v>
+        <v>5.7279999999999994E-4</v>
       </c>
       <c r="D21">
-        <v>1.6704999999999999E-3</v>
+        <v>2.0027000000000001E-3</v>
       </c>
       <c r="E21">
-        <v>4.7204000000000013E-3</v>
+        <v>7.7119000000000007E-3</v>
       </c>
       <c r="F21">
-        <v>1.7070599999999998E-2</v>
+        <v>2.932729999999999E-2</v>
       </c>
       <c r="G21">
-        <v>6.006725000000001E-3</v>
+        <v>9.9036749999999989E-3</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A22">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B22" t="s">
-        <v>58</v>
+        <v>27</v>
       </c>
       <c r="C22">
-        <v>2.9250000000000001E-4</v>
+        <v>5.6240000000000001E-4</v>
       </c>
       <c r="D22">
-        <v>9.6199999999999996E-4</v>
+        <v>2.2937000000000001E-3</v>
       </c>
       <c r="E22">
-        <v>3.9028000000000001E-3</v>
+        <v>8.2033999999999996E-3</v>
       </c>
       <c r="F22">
-        <v>1.89211E-2</v>
+        <v>3.1877699999999988E-2</v>
       </c>
       <c r="G22">
-        <v>6.0196000000000008E-3</v>
+        <v>1.07343E-2</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A23">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B23" t="s">
-        <v>42</v>
+        <v>28</v>
       </c>
       <c r="C23">
-        <v>3.9750000000000001E-4</v>
+        <v>8.7040000000000001E-4</v>
       </c>
       <c r="D23">
-        <v>1.2373E-3</v>
+        <v>4.7925999999999993E-3</v>
       </c>
       <c r="E23">
-        <v>4.0920000000000002E-3</v>
+        <v>3.0382299999999991E-2</v>
       </c>
       <c r="F23">
-        <v>1.8478899999999999E-2</v>
+        <v>0.1966658</v>
       </c>
       <c r="G23">
-        <v>6.051425E-3</v>
+        <v>5.8177775000000008E-2</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A24">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B24" t="s">
-        <v>68</v>
+        <v>29</v>
       </c>
       <c r="C24">
-        <v>3.3349999999999997E-4</v>
+        <v>5.5269999999999994E-4</v>
       </c>
       <c r="D24">
-        <v>1.0222E-3</v>
+        <v>2.5788E-3</v>
       </c>
       <c r="E24">
-        <v>3.9292999999999993E-3</v>
+        <v>1.1103399999999999E-2</v>
       </c>
       <c r="F24">
-        <v>1.9344500000000001E-2</v>
+        <v>5.6672599999999997E-2</v>
       </c>
       <c r="G24">
-        <v>6.1573749999999997E-3</v>
+        <v>1.7726875E-2</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A25">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B25" t="s">
-        <v>59</v>
+        <v>30</v>
       </c>
       <c r="C25">
-        <v>4.3370000000000003E-4</v>
+        <v>5.6940000000000007E-4</v>
       </c>
       <c r="D25">
-        <v>1.2313000000000001E-3</v>
+        <v>2.4130000000000002E-3</v>
       </c>
       <c r="E25">
-        <v>4.1329000000000001E-3</v>
+        <v>1.3361E-2</v>
       </c>
       <c r="F25">
-        <v>1.9089800000000001E-2</v>
+        <v>5.5955500000000012E-2</v>
       </c>
       <c r="G25">
-        <v>6.2219249999999997E-3</v>
+        <v>1.8074725E-2</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.3">
@@ -1200,68 +1200,68 @@
         <v>3</v>
       </c>
       <c r="B26" t="s">
-        <v>47</v>
+        <v>31</v>
       </c>
       <c r="C26">
-        <v>6.0229999999999995E-4</v>
+        <v>5.7199999999999992E-4</v>
       </c>
       <c r="D26">
-        <v>1.8128E-3</v>
+        <v>2.6386999999999999E-3</v>
       </c>
       <c r="E26">
-        <v>5.8475999999999997E-3</v>
+        <v>1.2478899999999999E-2</v>
       </c>
       <c r="F26">
-        <v>2.1591200000000001E-2</v>
+        <v>6.0133600000000002E-2</v>
       </c>
       <c r="G26">
-        <v>7.4634749999999989E-3</v>
+        <v>1.8955799999999998E-2</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A27">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B27" t="s">
-        <v>63</v>
+        <v>32</v>
       </c>
       <c r="C27">
-        <v>6.3679999999999997E-4</v>
+        <v>4.0089999999999988E-4</v>
       </c>
       <c r="D27">
-        <v>1.8515999999999999E-3</v>
+        <v>1.7438E-3</v>
       </c>
       <c r="E27">
-        <v>5.7964999999999996E-3</v>
+        <v>7.4894999999999996E-3</v>
       </c>
       <c r="F27">
-        <v>2.20091E-2</v>
+        <v>3.3035500000000002E-2</v>
       </c>
       <c r="G27">
-        <v>7.5735000000000004E-3</v>
+        <v>1.0667424999999999E-2</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A28">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B28" t="s">
-        <v>25</v>
+        <v>33</v>
       </c>
       <c r="C28">
-        <v>5.9829999999999996E-4</v>
+        <v>4.2719999999999998E-4</v>
       </c>
       <c r="D28">
-        <v>1.7952000000000001E-3</v>
+        <v>1.7413999999999999E-3</v>
       </c>
       <c r="E28">
-        <v>6.3026999999999996E-3</v>
+        <v>7.4197000000000004E-3</v>
       </c>
       <c r="F28">
-        <v>2.30758E-2</v>
+        <v>3.2341699999999987E-2</v>
       </c>
       <c r="G28">
-        <v>7.9430000000000004E-3</v>
+        <v>1.04825E-2</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.3">
@@ -1269,137 +1269,137 @@
         <v>3</v>
       </c>
       <c r="B29" t="s">
-        <v>46</v>
+        <v>34</v>
       </c>
       <c r="C29">
-        <v>6.198E-4</v>
+        <v>4.7980000000000001E-4</v>
       </c>
       <c r="D29">
-        <v>1.8263000000000001E-3</v>
+        <v>2.0875999999999998E-3</v>
       </c>
       <c r="E29">
-        <v>6.4658000000000007E-3</v>
+        <v>7.1725999999999986E-3</v>
       </c>
       <c r="F29">
-        <v>2.3189999999999999E-2</v>
+        <v>2.9955900000000001E-2</v>
       </c>
       <c r="G29">
-        <v>8.0254750000000007E-3</v>
+        <v>9.9239749999999998E-3</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A30">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B30" t="s">
-        <v>8</v>
+        <v>35</v>
       </c>
       <c r="C30">
-        <v>3.9439999999999988E-4</v>
+        <v>1.0307999999999999E-3</v>
       </c>
       <c r="D30">
-        <v>1.5790000000000001E-3</v>
+        <v>4.8712E-3</v>
       </c>
       <c r="E30">
-        <v>6.460200000000001E-3</v>
+        <v>3.0890299999999999E-2</v>
       </c>
       <c r="F30">
-        <v>2.7491499999999999E-2</v>
+        <v>0.19775970000000001</v>
       </c>
       <c r="G30">
-        <v>8.9812750000000004E-3</v>
+        <v>5.8638000000000003E-2</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A31">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B31" t="s">
-        <v>16</v>
+        <v>36</v>
       </c>
       <c r="C31">
-        <v>4.4660000000000001E-4</v>
+        <v>1.0204000000000001E-3</v>
       </c>
       <c r="D31">
-        <v>1.6946000000000001E-3</v>
+        <v>5.8806000000000006E-3</v>
       </c>
       <c r="E31">
-        <v>6.8047999999999997E-3</v>
+        <v>3.4577200000000002E-2</v>
       </c>
       <c r="F31">
-        <v>2.8878500000000001E-2</v>
+        <v>0.22706989999999999</v>
       </c>
       <c r="G31">
-        <v>9.4561249999999993E-3</v>
+        <v>6.7137024999999989E-2</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A32">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B32" t="s">
-        <v>17</v>
+        <v>37</v>
       </c>
       <c r="C32">
-        <v>4.37E-4</v>
+        <v>1.0491000000000001E-3</v>
       </c>
       <c r="D32">
-        <v>1.8249E-3</v>
+        <v>5.8165999999999999E-3</v>
       </c>
       <c r="E32">
-        <v>7.0086000000000011E-3</v>
+        <v>3.3596599999999997E-2</v>
       </c>
       <c r="F32">
-        <v>2.96522E-2</v>
+        <v>0.22013679999999999</v>
       </c>
       <c r="G32">
-        <v>9.7306750000000011E-3</v>
+        <v>6.5149774999999993E-2</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A33">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B33" t="s">
-        <v>11</v>
+        <v>38</v>
       </c>
       <c r="C33">
-        <v>5.4959999999999991E-4</v>
+        <v>8.7679999999999995E-4</v>
       </c>
       <c r="D33">
-        <v>2.0154999999999999E-3</v>
+        <v>4.5497999999999997E-3</v>
       </c>
       <c r="E33">
-        <v>7.6709999999999999E-3</v>
+        <v>2.6851400000000001E-2</v>
       </c>
       <c r="F33">
-        <v>2.8932099999999999E-2</v>
+        <v>0.167374</v>
       </c>
       <c r="G33">
-        <v>9.7920500000000001E-3</v>
+        <v>4.9912999999999999E-2</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A34">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B34" t="s">
-        <v>26</v>
+        <v>39</v>
       </c>
       <c r="C34">
-        <v>5.7279999999999994E-4</v>
+        <v>4.3110000000000002E-4</v>
       </c>
       <c r="D34">
-        <v>2.0027000000000001E-3</v>
+        <v>1.3385000000000001E-3</v>
       </c>
       <c r="E34">
-        <v>7.7119000000000007E-3</v>
+        <v>4.0620000000000014E-3</v>
       </c>
       <c r="F34">
-        <v>2.932729999999999E-2</v>
+        <v>1.4038999999999999E-2</v>
       </c>
       <c r="G34">
-        <v>9.9036749999999989E-3</v>
+        <v>4.9676500000000014E-3</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.3">
@@ -1407,45 +1407,45 @@
         <v>3</v>
       </c>
       <c r="B35" t="s">
-        <v>34</v>
+        <v>40</v>
       </c>
       <c r="C35">
-        <v>4.7980000000000001E-4</v>
+        <v>2.6330000000000011E-4</v>
       </c>
       <c r="D35">
-        <v>2.0875999999999998E-3</v>
+        <v>8.7900000000000012E-4</v>
       </c>
       <c r="E35">
-        <v>7.1725999999999986E-3</v>
+        <v>2.932300000000001E-3</v>
       </c>
       <c r="F35">
-        <v>2.9955900000000001E-2</v>
+        <v>1.0929700000000001E-2</v>
       </c>
       <c r="G35">
-        <v>9.9239749999999998E-3</v>
+        <v>3.751075E-3</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A36">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B36" t="s">
-        <v>15</v>
+        <v>41</v>
       </c>
       <c r="C36">
-        <v>3.5E-4</v>
+        <v>4.7790000000000002E-4</v>
       </c>
       <c r="D36">
-        <v>1.6364999999999999E-3</v>
+        <v>1.5106E-3</v>
       </c>
       <c r="E36">
-        <v>7.0992E-3</v>
+        <v>4.8173999999999986E-3</v>
       </c>
       <c r="F36">
-        <v>3.1927499999999998E-2</v>
+        <v>1.68845E-2</v>
       </c>
       <c r="G36">
-        <v>1.02533E-2</v>
+        <v>5.9226000000000001E-3</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.3">
@@ -1453,22 +1453,22 @@
         <v>3</v>
       </c>
       <c r="B37" t="s">
-        <v>33</v>
+        <v>42</v>
       </c>
       <c r="C37">
-        <v>4.2719999999999998E-4</v>
+        <v>3.9750000000000001E-4</v>
       </c>
       <c r="D37">
-        <v>1.7413999999999999E-3</v>
+        <v>1.2373E-3</v>
       </c>
       <c r="E37">
-        <v>7.4197000000000004E-3</v>
+        <v>4.0920000000000002E-3</v>
       </c>
       <c r="F37">
-        <v>3.2341699999999987E-2</v>
+        <v>1.8478899999999999E-2</v>
       </c>
       <c r="G37">
-        <v>1.04825E-2</v>
+        <v>6.051425E-3</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.3">
@@ -1476,68 +1476,68 @@
         <v>3</v>
       </c>
       <c r="B38" t="s">
-        <v>32</v>
+        <v>43</v>
       </c>
       <c r="C38">
-        <v>4.0089999999999988E-4</v>
+        <v>5.0170000000000011E-4</v>
       </c>
       <c r="D38">
-        <v>1.7438E-3</v>
+        <v>1.606E-3</v>
       </c>
       <c r="E38">
-        <v>7.4894999999999996E-3</v>
+        <v>4.5802000000000004E-3</v>
       </c>
       <c r="F38">
-        <v>3.3035500000000002E-2</v>
+        <v>1.54742E-2</v>
       </c>
       <c r="G38">
-        <v>1.0667424999999999E-2</v>
+        <v>5.5405250000000001E-3</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A39">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B39" t="s">
-        <v>27</v>
+        <v>44</v>
       </c>
       <c r="C39">
-        <v>5.6240000000000001E-4</v>
+        <v>4.6989999999999988E-4</v>
       </c>
       <c r="D39">
-        <v>2.2937000000000001E-3</v>
+        <v>1.4894999999999999E-3</v>
       </c>
       <c r="E39">
-        <v>8.2033999999999996E-3</v>
+        <v>4.9845000000000002E-3</v>
       </c>
       <c r="F39">
-        <v>3.1877699999999988E-2</v>
+        <v>1.31269E-2</v>
       </c>
       <c r="G39">
-        <v>1.07343E-2</v>
+        <v>5.0177000000000008E-3</v>
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A40">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B40" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
       <c r="C40">
-        <v>4.5679999999999999E-4</v>
+        <v>4.975E-4</v>
       </c>
       <c r="D40">
-        <v>1.9105000000000001E-3</v>
+        <v>1.5995E-3</v>
       </c>
       <c r="E40">
-        <v>7.7654999999999998E-3</v>
+        <v>4.5439000000000009E-3</v>
       </c>
       <c r="F40">
-        <v>3.3472600000000012E-2</v>
+        <v>1.70324E-2</v>
       </c>
       <c r="G40">
-        <v>1.0901350000000001E-2</v>
+        <v>5.9183250000000012E-3</v>
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.3">
@@ -1545,45 +1545,45 @@
         <v>3</v>
       </c>
       <c r="B41" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C41">
-        <v>5.8700000000000007E-4</v>
+        <v>6.198E-4</v>
       </c>
       <c r="D41">
-        <v>2.2431999999999999E-3</v>
+        <v>1.8263000000000001E-3</v>
       </c>
       <c r="E41">
-        <v>8.3339E-3</v>
+        <v>6.4658000000000007E-3</v>
       </c>
       <c r="F41">
-        <v>3.3125099999999998E-2</v>
+        <v>2.3189999999999999E-2</v>
       </c>
       <c r="G41">
-        <v>1.10723E-2</v>
+        <v>8.0254750000000007E-3</v>
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A42">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B42" t="s">
-        <v>14</v>
+        <v>47</v>
       </c>
       <c r="C42">
-        <v>5.1900000000000004E-4</v>
+        <v>6.0229999999999995E-4</v>
       </c>
       <c r="D42">
-        <v>2.5062999999999999E-3</v>
+        <v>1.8128E-3</v>
       </c>
       <c r="E42">
-        <v>1.0818299999999999E-2</v>
+        <v>5.8475999999999997E-3</v>
       </c>
       <c r="F42">
-        <v>5.5259999999999997E-2</v>
+        <v>2.1591200000000001E-2</v>
       </c>
       <c r="G42">
-        <v>1.72759E-2</v>
+        <v>7.4634749999999989E-3</v>
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.3">
@@ -1591,45 +1591,45 @@
         <v>3</v>
       </c>
       <c r="B43" t="s">
-        <v>29</v>
+        <v>48</v>
       </c>
       <c r="C43">
-        <v>5.5269999999999994E-4</v>
+        <v>5.8700000000000007E-4</v>
       </c>
       <c r="D43">
-        <v>2.5788E-3</v>
+        <v>2.2431999999999999E-3</v>
       </c>
       <c r="E43">
-        <v>1.1103399999999999E-2</v>
+        <v>8.3339E-3</v>
       </c>
       <c r="F43">
-        <v>5.6672599999999997E-2</v>
+        <v>3.3125099999999998E-2</v>
       </c>
       <c r="G43">
-        <v>1.7726875E-2</v>
+        <v>1.10723E-2</v>
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A44">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B44" t="s">
-        <v>30</v>
+        <v>49</v>
       </c>
       <c r="C44">
-        <v>5.6940000000000007E-4</v>
+        <v>6.3170000000000001E-4</v>
       </c>
       <c r="D44">
-        <v>2.4130000000000002E-3</v>
+        <v>2.6078E-3</v>
       </c>
       <c r="E44">
-        <v>1.3361E-2</v>
+        <v>1.24546E-2</v>
       </c>
       <c r="F44">
-        <v>5.5955500000000012E-2</v>
+        <v>5.67871E-2</v>
       </c>
       <c r="G44">
-        <v>1.8074725E-2</v>
+        <v>1.8120299999999999E-2</v>
       </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.3">
@@ -1637,22 +1637,22 @@
         <v>4</v>
       </c>
       <c r="B45" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C45">
-        <v>5.7959999999999989E-4</v>
+        <v>5.8759999999999997E-4</v>
       </c>
       <c r="D45">
-        <v>2.7095999999999999E-3</v>
+        <v>2.8303E-3</v>
       </c>
       <c r="E45">
-        <v>1.1530200000000001E-2</v>
+        <v>1.22928E-2</v>
       </c>
       <c r="F45">
-        <v>5.7557099999999993E-2</v>
+        <v>6.0997100000000012E-2</v>
       </c>
       <c r="G45">
-        <v>1.8094124999999999E-2</v>
+        <v>1.9176950000000002E-2</v>
       </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.3">
@@ -1660,68 +1660,68 @@
         <v>4</v>
       </c>
       <c r="B46" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="C46">
-        <v>6.3170000000000001E-4</v>
+        <v>5.7959999999999989E-4</v>
       </c>
       <c r="D46">
-        <v>2.6078E-3</v>
+        <v>2.7095999999999999E-3</v>
       </c>
       <c r="E46">
-        <v>1.24546E-2</v>
+        <v>1.1530200000000001E-2</v>
       </c>
       <c r="F46">
-        <v>5.67871E-2</v>
+        <v>5.7557099999999993E-2</v>
       </c>
       <c r="G46">
-        <v>1.8120299999999999E-2</v>
+        <v>1.8094124999999999E-2</v>
       </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A47">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B47" t="s">
-        <v>64</v>
+        <v>52</v>
       </c>
       <c r="C47">
-        <v>6.4560000000000008E-4</v>
+        <v>4.5679999999999999E-4</v>
       </c>
       <c r="D47">
-        <v>2.8408000000000001E-3</v>
+        <v>1.9105000000000001E-3</v>
       </c>
       <c r="E47">
-        <v>1.2025599999999999E-2</v>
+        <v>7.7654999999999998E-3</v>
       </c>
       <c r="F47">
-        <v>5.8474999999999999E-2</v>
+        <v>3.3472600000000012E-2</v>
       </c>
       <c r="G47">
-        <v>1.8496749999999999E-2</v>
+        <v>1.0901350000000001E-2</v>
       </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A48">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B48" t="s">
-        <v>31</v>
+        <v>53</v>
       </c>
       <c r="C48">
-        <v>5.7199999999999992E-4</v>
+        <v>1.1359E-3</v>
       </c>
       <c r="D48">
-        <v>2.6386999999999999E-3</v>
+        <v>6.0593000000000001E-3</v>
       </c>
       <c r="E48">
-        <v>1.2478899999999999E-2</v>
+        <v>3.4112900000000002E-2</v>
       </c>
       <c r="F48">
-        <v>6.0133600000000002E-2</v>
+        <v>0.2212797</v>
       </c>
       <c r="G48">
-        <v>1.8955799999999998E-2</v>
+        <v>6.5646950000000009E-2</v>
       </c>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.3">
@@ -1729,398 +1729,403 @@
         <v>4</v>
       </c>
       <c r="B49" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="C49">
-        <v>5.8759999999999997E-4</v>
+        <v>4.8069999999999997E-4</v>
       </c>
       <c r="D49">
-        <v>2.8303E-3</v>
+        <v>1.3879999999999999E-3</v>
       </c>
       <c r="E49">
-        <v>1.22928E-2</v>
+        <v>4.1368000000000004E-3</v>
       </c>
       <c r="F49">
-        <v>6.0997100000000012E-2</v>
+        <v>1.4173099999999999E-2</v>
       </c>
       <c r="G49">
-        <v>1.9176950000000002E-2</v>
+        <v>5.0446499999999986E-3</v>
       </c>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A50">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B50" t="s">
-        <v>22</v>
+        <v>55</v>
       </c>
       <c r="C50">
-        <v>8.4049999999999988E-4</v>
+        <v>4.4200000000000001E-4</v>
       </c>
       <c r="D50">
-        <v>4.4665E-3</v>
+        <v>1.3045999999999999E-3</v>
       </c>
       <c r="E50">
-        <v>2.62738E-2</v>
+        <v>3.9623000000000002E-3</v>
       </c>
       <c r="F50">
-        <v>0.1665604</v>
+        <v>1.54468E-2</v>
       </c>
       <c r="G50">
-        <v>4.9535299999999997E-2</v>
+        <v>5.2889249999999999E-3</v>
       </c>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A51">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B51" t="s">
-        <v>38</v>
+        <v>56</v>
       </c>
       <c r="C51">
-        <v>8.7679999999999995E-4</v>
+        <v>3.3599999999999998E-4</v>
       </c>
       <c r="D51">
-        <v>4.5497999999999997E-3</v>
+        <v>9.6270000000000004E-4</v>
       </c>
       <c r="E51">
-        <v>2.6851400000000001E-2</v>
+        <v>2.9889999999999999E-3</v>
       </c>
       <c r="F51">
-        <v>0.167374</v>
+        <v>1.1006200000000001E-2</v>
       </c>
       <c r="G51">
-        <v>4.9912999999999999E-2</v>
+        <v>3.8234749999999998E-3</v>
       </c>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A52">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="B52" t="s">
-        <v>10</v>
+        <v>57</v>
       </c>
       <c r="C52">
-        <v>8.0180000000000008E-4</v>
+        <v>3.1470000000000001E-4</v>
       </c>
       <c r="D52">
-        <v>4.1804999999999993E-3</v>
+        <v>1.0001999999999999E-3</v>
       </c>
       <c r="E52">
-        <v>2.69538E-2</v>
+        <v>3.0230999999999999E-3</v>
       </c>
       <c r="F52">
-        <v>0.17773829999999999</v>
+        <v>1.1051200000000001E-2</v>
       </c>
       <c r="G52">
-        <v>5.2418600000000003E-2</v>
+        <v>3.8473000000000001E-3</v>
       </c>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A53">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B53" t="s">
-        <v>21</v>
+        <v>58</v>
       </c>
       <c r="C53">
-        <v>8.4270000000000005E-4</v>
+        <v>2.9250000000000001E-4</v>
       </c>
       <c r="D53">
-        <v>4.4114000000000002E-3</v>
+        <v>9.6199999999999996E-4</v>
       </c>
       <c r="E53">
-        <v>2.77015E-2</v>
+        <v>3.9028000000000001E-3</v>
       </c>
       <c r="F53">
-        <v>0.17886940000000001</v>
+        <v>1.89211E-2</v>
       </c>
       <c r="G53">
-        <v>5.2956250000000003E-2</v>
+        <v>6.0196000000000008E-3</v>
       </c>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A54">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B54" t="s">
-        <v>18</v>
+        <v>59</v>
       </c>
       <c r="C54">
-        <v>9.1180000000000015E-4</v>
+        <v>4.3370000000000003E-4</v>
       </c>
       <c r="D54">
-        <v>4.4942999999999997E-3</v>
+        <v>1.2313000000000001E-3</v>
       </c>
       <c r="E54">
-        <v>2.8027300000000002E-2</v>
+        <v>4.1329000000000001E-3</v>
       </c>
       <c r="F54">
-        <v>0.17958470000000001</v>
+        <v>1.9089800000000001E-2</v>
       </c>
       <c r="G54">
-        <v>5.3254524999999997E-2</v>
+        <v>6.2219249999999997E-3</v>
       </c>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A55">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="B55" t="s">
-        <v>9</v>
+        <v>60</v>
       </c>
       <c r="C55">
-        <v>8.7399999999999999E-4</v>
+        <v>5.2250000000000007E-4</v>
       </c>
       <c r="D55">
-        <v>4.3349E-3</v>
+        <v>1.5704E-3</v>
       </c>
       <c r="E55">
-        <v>2.7797499999999999E-2</v>
+        <v>3.9540999999999986E-3</v>
       </c>
       <c r="F55">
-        <v>0.18007819999999999</v>
+        <v>1.35342E-2</v>
       </c>
       <c r="G55">
-        <v>5.3271150000000003E-2</v>
+        <v>4.8953E-3</v>
       </c>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A56">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="B56" t="s">
-        <v>13</v>
+        <v>61</v>
       </c>
       <c r="C56">
-        <v>8.3429999999999995E-4</v>
+        <v>5.6980000000000008E-4</v>
       </c>
       <c r="D56">
-        <v>4.7235999999999997E-3</v>
+        <v>1.6581E-3</v>
       </c>
       <c r="E56">
-        <v>3.0702199999999999E-2</v>
+        <v>4.6348000000000014E-3</v>
       </c>
       <c r="F56">
-        <v>0.195657</v>
+        <v>1.7063499999999999E-2</v>
       </c>
       <c r="G56">
-        <v>5.7979274999999997E-2</v>
+        <v>5.9815500000000004E-3</v>
       </c>
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A57">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B57" t="s">
-        <v>28</v>
+        <v>62</v>
       </c>
       <c r="C57">
-        <v>8.7040000000000001E-4</v>
+        <v>5.1840000000000002E-4</v>
       </c>
       <c r="D57">
-        <v>4.7925999999999993E-3</v>
+        <v>1.6442E-3</v>
       </c>
       <c r="E57">
-        <v>3.0382299999999991E-2</v>
+        <v>4.5433000000000001E-3</v>
       </c>
       <c r="F57">
-        <v>0.1966658</v>
+        <v>1.68763E-2</v>
       </c>
       <c r="G57">
-        <v>5.8177775000000008E-2</v>
+        <v>5.8955500000000011E-3</v>
       </c>
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A58">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="B58" t="s">
-        <v>7</v>
+        <v>63</v>
       </c>
       <c r="C58">
-        <v>7.9670000000000001E-4</v>
+        <v>6.3679999999999997E-4</v>
       </c>
       <c r="D58">
-        <v>4.4444999999999997E-3</v>
+        <v>1.8515999999999999E-3</v>
       </c>
       <c r="E58">
-        <v>2.9551299999999999E-2</v>
+        <v>5.7964999999999996E-3</v>
       </c>
       <c r="F58">
-        <v>0.19877359999999999</v>
+        <v>2.20091E-2</v>
       </c>
       <c r="G58">
-        <v>5.8391524999999993E-2</v>
+        <v>7.5735000000000004E-3</v>
       </c>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A59">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B59" t="s">
-        <v>35</v>
+        <v>64</v>
       </c>
       <c r="C59">
-        <v>1.0307999999999999E-3</v>
+        <v>6.4560000000000008E-4</v>
       </c>
       <c r="D59">
-        <v>4.8712E-3</v>
+        <v>2.8408000000000001E-3</v>
       </c>
       <c r="E59">
-        <v>3.0890299999999999E-2</v>
+        <v>1.2025599999999999E-2</v>
       </c>
       <c r="F59">
-        <v>0.19775970000000001</v>
+        <v>5.8474999999999999E-2</v>
       </c>
       <c r="G59">
-        <v>5.8638000000000003E-2</v>
+        <v>1.8496749999999999E-2</v>
       </c>
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A60">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="B60" t="s">
-        <v>19</v>
+        <v>65</v>
       </c>
       <c r="C60">
-        <v>9.9789999999999992E-4</v>
+        <v>4.8720000000000002E-4</v>
       </c>
       <c r="D60">
-        <v>4.7220999999999999E-3</v>
+        <v>1.4147999999999999E-3</v>
       </c>
       <c r="E60">
-        <v>3.1725499999999997E-2</v>
+        <v>4.1064000000000014E-3</v>
       </c>
       <c r="F60">
-        <v>0.19733619999999999</v>
+        <v>1.5676499999999999E-2</v>
       </c>
       <c r="G60">
-        <v>5.8695425000000009E-2</v>
+        <v>5.421225E-3</v>
       </c>
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A61">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="B61" t="s">
-        <v>12</v>
+        <v>66</v>
       </c>
       <c r="C61">
-        <v>8.183000000000001E-4</v>
+        <v>3.8249999999999997E-4</v>
       </c>
       <c r="D61">
-        <v>4.5246000000000001E-3</v>
+        <v>1.0116999999999999E-3</v>
       </c>
       <c r="E61">
-        <v>3.0049900000000001E-2</v>
+        <v>3.2128E-3</v>
       </c>
       <c r="F61">
-        <v>0.20457220000000001</v>
+        <v>1.11264E-2</v>
       </c>
       <c r="G61">
-        <v>5.9991250000000003E-2</v>
+        <v>3.9333500000000004E-3</v>
       </c>
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A62">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B62" t="s">
-        <v>37</v>
+        <v>67</v>
       </c>
       <c r="C62">
-        <v>1.0491000000000001E-3</v>
+        <v>3.6549999999999999E-4</v>
       </c>
       <c r="D62">
-        <v>5.8165999999999999E-3</v>
+        <v>1.0134E-3</v>
       </c>
       <c r="E62">
-        <v>3.3596599999999997E-2</v>
+        <v>3.6587E-3</v>
       </c>
       <c r="F62">
-        <v>0.22013679999999999</v>
+        <v>1.7533699999999999E-2</v>
       </c>
       <c r="G62">
-        <v>6.5149774999999993E-2</v>
+        <v>5.6428249999999998E-3</v>
       </c>
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A63">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B63" t="s">
-        <v>53</v>
+        <v>68</v>
       </c>
       <c r="C63">
-        <v>1.1359E-3</v>
+        <v>3.3349999999999997E-4</v>
       </c>
       <c r="D63">
-        <v>6.0593000000000001E-3</v>
+        <v>1.0222E-3</v>
       </c>
       <c r="E63">
-        <v>3.4112900000000002E-2</v>
+        <v>3.9292999999999993E-3</v>
       </c>
       <c r="F63">
-        <v>0.2212797</v>
+        <v>1.9344500000000001E-2</v>
       </c>
       <c r="G63">
-        <v>6.5646950000000009E-2</v>
+        <v>6.1573749999999997E-3</v>
       </c>
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A64">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="B64" t="s">
-        <v>20</v>
+        <v>69</v>
       </c>
       <c r="C64">
-        <v>1.005E-3</v>
+        <v>5.6540000000000008E-4</v>
       </c>
       <c r="D64">
-        <v>5.6778999999999996E-3</v>
+        <v>1.6704999999999999E-3</v>
       </c>
       <c r="E64">
-        <v>3.4527299999999997E-2</v>
+        <v>4.7204000000000013E-3</v>
       </c>
       <c r="F64">
-        <v>0.225498</v>
+        <v>1.7070599999999998E-2</v>
       </c>
       <c r="G64">
-        <v>6.6677049999999988E-2</v>
+        <v>6.006725000000001E-3</v>
       </c>
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A65">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="B65" t="s">
-        <v>36</v>
+        <v>70</v>
       </c>
       <c r="C65">
-        <v>1.0204000000000001E-3</v>
+        <v>3.9350000000000002E-4</v>
       </c>
       <c r="D65">
-        <v>5.8806000000000006E-3</v>
+        <v>1.0667999999999999E-3</v>
       </c>
       <c r="E65">
-        <v>3.4577200000000002E-2</v>
+        <v>3.7215E-3</v>
       </c>
       <c r="F65">
-        <v>0.22706989999999999</v>
+        <v>1.7754800000000001E-2</v>
       </c>
       <c r="G65">
-        <v>6.7137024999999989E-2</v>
+        <v>5.7341500000000004E-3</v>
       </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:G65" xr:uid="{00000000-0001-0000-0000-000000000000}">
     <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G65">
-      <sortCondition ref="G1:G65"/>
+      <sortCondition ref="A2:A65"/>
+      <sortCondition ref="B2:B65"/>
     </sortState>
   </autoFilter>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G7">
+    <sortCondition ref="A2:A7"/>
+    <sortCondition ref="B2:B7"/>
+  </sortState>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
Algoritma dengan ketahanan terbaik JPS BDS GL BRC PPO
</commit_message>
<xml_diff>
--- a/Excel/Hasil_Pengujian_Map_128_avg_length.xlsx
+++ b/Excel/Hasil_Pengujian_Map_128_avg_length.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\SEMHAS\TA_Python_Server\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E164595-A15D-45E7-B844-F330DAC781A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49F107CB-3D82-42BE-96CC-936E301559ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -610,8 +610,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G65"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:F8"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2:G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -694,22 +694,22 @@
         <v>1</v>
       </c>
       <c r="B4" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="C4">
-        <v>8.7399999999999999E-4</v>
+        <v>5.4959999999999991E-4</v>
       </c>
       <c r="D4">
-        <v>4.3349E-3</v>
+        <v>2.0154999999999999E-3</v>
       </c>
       <c r="E4">
-        <v>2.7797499999999999E-2</v>
+        <v>7.6709999999999999E-3</v>
       </c>
       <c r="F4">
-        <v>0.18007819999999999</v>
+        <v>2.8932099999999999E-2</v>
       </c>
       <c r="G4">
-        <v>5.3271150000000003E-2</v>
+        <v>9.7920500000000001E-3</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
@@ -740,22 +740,22 @@
         <v>1</v>
       </c>
       <c r="B6" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C6">
-        <v>5.4959999999999991E-4</v>
+        <v>8.7399999999999999E-4</v>
       </c>
       <c r="D6">
-        <v>2.0154999999999999E-3</v>
+        <v>4.3349E-3</v>
       </c>
       <c r="E6">
-        <v>7.6709999999999999E-3</v>
+        <v>2.7797499999999999E-2</v>
       </c>
       <c r="F6">
-        <v>2.8932099999999999E-2</v>
+        <v>0.18007819999999999</v>
       </c>
       <c r="G6">
-        <v>9.7920500000000001E-3</v>
+        <v>5.3271150000000003E-2</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
@@ -763,22 +763,22 @@
         <v>1</v>
       </c>
       <c r="B7" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C7">
-        <v>8.183000000000001E-4</v>
+        <v>8.3429999999999995E-4</v>
       </c>
       <c r="D7">
-        <v>4.5246000000000001E-3</v>
+        <v>4.7235999999999997E-3</v>
       </c>
       <c r="E7">
-        <v>3.0049900000000001E-2</v>
+        <v>3.0702199999999999E-2</v>
       </c>
       <c r="F7">
-        <v>0.20457220000000001</v>
+        <v>0.195657</v>
       </c>
       <c r="G7">
-        <v>5.9991250000000003E-2</v>
+        <v>5.7979274999999997E-2</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
@@ -786,22 +786,22 @@
         <v>1</v>
       </c>
       <c r="B8" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C8">
-        <v>8.3429999999999995E-4</v>
+        <v>8.183000000000001E-4</v>
       </c>
       <c r="D8">
-        <v>4.7235999999999997E-3</v>
+        <v>4.5246000000000001E-3</v>
       </c>
       <c r="E8">
-        <v>3.0702199999999999E-2</v>
+        <v>3.0049900000000001E-2</v>
       </c>
       <c r="F8">
-        <v>0.195657</v>
+        <v>0.20457220000000001</v>
       </c>
       <c r="G8">
-        <v>5.7979274999999997E-2</v>
+        <v>5.9991250000000003E-2</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
@@ -809,22 +809,22 @@
         <v>2</v>
       </c>
       <c r="B9" t="s">
-        <v>14</v>
+        <v>24</v>
       </c>
       <c r="C9">
-        <v>5.1900000000000004E-4</v>
+        <v>4.7279999999999989E-4</v>
       </c>
       <c r="D9">
-        <v>2.5062999999999999E-3</v>
+        <v>1.5681E-3</v>
       </c>
       <c r="E9">
-        <v>1.0818299999999999E-2</v>
+        <v>4.6663E-3</v>
       </c>
       <c r="F9">
-        <v>5.5259999999999997E-2</v>
+        <v>1.51979E-2</v>
       </c>
       <c r="G9">
-        <v>1.72759E-2</v>
+        <v>5.4762749999999992E-3</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
@@ -832,22 +832,22 @@
         <v>2</v>
       </c>
       <c r="B10" t="s">
-        <v>15</v>
+        <v>23</v>
       </c>
       <c r="C10">
-        <v>3.5E-4</v>
+        <v>4.3209999999999999E-4</v>
       </c>
       <c r="D10">
-        <v>1.6364999999999999E-3</v>
+        <v>1.4465000000000001E-3</v>
       </c>
       <c r="E10">
-        <v>7.0992E-3</v>
+        <v>4.7888999999999996E-3</v>
       </c>
       <c r="F10">
-        <v>3.1927499999999998E-2</v>
+        <v>1.6785999999999999E-2</v>
       </c>
       <c r="G10">
-        <v>1.02533E-2</v>
+        <v>5.8633750000000014E-3</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
@@ -855,22 +855,22 @@
         <v>2</v>
       </c>
       <c r="B11" t="s">
-        <v>16</v>
+        <v>25</v>
       </c>
       <c r="C11">
-        <v>4.4660000000000001E-4</v>
+        <v>5.9829999999999996E-4</v>
       </c>
       <c r="D11">
-        <v>1.6946000000000001E-3</v>
+        <v>1.7952000000000001E-3</v>
       </c>
       <c r="E11">
-        <v>6.8047999999999997E-3</v>
+        <v>6.3026999999999996E-3</v>
       </c>
       <c r="F11">
-        <v>2.8878500000000001E-2</v>
+        <v>2.30758E-2</v>
       </c>
       <c r="G11">
-        <v>9.4561249999999993E-3</v>
+        <v>7.9430000000000004E-3</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
@@ -878,22 +878,22 @@
         <v>2</v>
       </c>
       <c r="B12" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C12">
-        <v>4.37E-4</v>
+        <v>4.4660000000000001E-4</v>
       </c>
       <c r="D12">
-        <v>1.8249E-3</v>
+        <v>1.6946000000000001E-3</v>
       </c>
       <c r="E12">
-        <v>7.0086000000000011E-3</v>
+        <v>6.8047999999999997E-3</v>
       </c>
       <c r="F12">
-        <v>2.96522E-2</v>
+        <v>2.8878500000000001E-2</v>
       </c>
       <c r="G12">
-        <v>9.7306750000000011E-3</v>
+        <v>9.4561249999999993E-3</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
@@ -901,22 +901,22 @@
         <v>2</v>
       </c>
       <c r="B13" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C13">
-        <v>9.1180000000000015E-4</v>
+        <v>4.37E-4</v>
       </c>
       <c r="D13">
-        <v>4.4942999999999997E-3</v>
+        <v>1.8249E-3</v>
       </c>
       <c r="E13">
-        <v>2.8027300000000002E-2</v>
+        <v>7.0086000000000011E-3</v>
       </c>
       <c r="F13">
-        <v>0.17958470000000001</v>
+        <v>2.96522E-2</v>
       </c>
       <c r="G13">
-        <v>5.3254524999999997E-2</v>
+        <v>9.7306750000000011E-3</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
@@ -924,22 +924,22 @@
         <v>2</v>
       </c>
       <c r="B14" t="s">
-        <v>19</v>
+        <v>26</v>
       </c>
       <c r="C14">
-        <v>9.9789999999999992E-4</v>
+        <v>5.7279999999999994E-4</v>
       </c>
       <c r="D14">
-        <v>4.7220999999999999E-3</v>
+        <v>2.0027000000000001E-3</v>
       </c>
       <c r="E14">
-        <v>3.1725499999999997E-2</v>
+        <v>7.7119000000000007E-3</v>
       </c>
       <c r="F14">
-        <v>0.19733619999999999</v>
+        <v>2.932729999999999E-2</v>
       </c>
       <c r="G14">
-        <v>5.8695425000000009E-2</v>
+        <v>9.9036749999999989E-3</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.3">
@@ -947,22 +947,22 @@
         <v>2</v>
       </c>
       <c r="B15" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="C15">
-        <v>1.005E-3</v>
+        <v>3.5E-4</v>
       </c>
       <c r="D15">
-        <v>5.6778999999999996E-3</v>
+        <v>1.6364999999999999E-3</v>
       </c>
       <c r="E15">
-        <v>3.4527299999999997E-2</v>
+        <v>7.0992E-3</v>
       </c>
       <c r="F15">
-        <v>0.225498</v>
+        <v>3.1927499999999998E-2</v>
       </c>
       <c r="G15">
-        <v>6.6677049999999988E-2</v>
+        <v>1.02533E-2</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.3">
@@ -970,22 +970,22 @@
         <v>2</v>
       </c>
       <c r="B16" t="s">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="C16">
-        <v>8.4270000000000005E-4</v>
+        <v>5.6240000000000001E-4</v>
       </c>
       <c r="D16">
-        <v>4.4114000000000002E-3</v>
+        <v>2.2937000000000001E-3</v>
       </c>
       <c r="E16">
-        <v>2.77015E-2</v>
+        <v>8.2033999999999996E-3</v>
       </c>
       <c r="F16">
-        <v>0.17886940000000001</v>
+        <v>3.1877699999999988E-2</v>
       </c>
       <c r="G16">
-        <v>5.2956250000000003E-2</v>
+        <v>1.07343E-2</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.3">
@@ -993,22 +993,22 @@
         <v>2</v>
       </c>
       <c r="B17" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="C17">
-        <v>8.4049999999999988E-4</v>
+        <v>5.1900000000000004E-4</v>
       </c>
       <c r="D17">
-        <v>4.4665E-3</v>
+        <v>2.5062999999999999E-3</v>
       </c>
       <c r="E17">
-        <v>2.62738E-2</v>
+        <v>1.0818299999999999E-2</v>
       </c>
       <c r="F17">
-        <v>0.1665604</v>
+        <v>5.5259999999999997E-2</v>
       </c>
       <c r="G17">
-        <v>4.9535299999999997E-2</v>
+        <v>1.72759E-2</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.3">
@@ -1016,22 +1016,22 @@
         <v>2</v>
       </c>
       <c r="B18" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C18">
-        <v>4.3209999999999999E-4</v>
+        <v>8.4049999999999988E-4</v>
       </c>
       <c r="D18">
-        <v>1.4465000000000001E-3</v>
+        <v>4.4665E-3</v>
       </c>
       <c r="E18">
-        <v>4.7888999999999996E-3</v>
+        <v>2.62738E-2</v>
       </c>
       <c r="F18">
-        <v>1.6785999999999999E-2</v>
+        <v>0.1665604</v>
       </c>
       <c r="G18">
-        <v>5.8633750000000014E-3</v>
+        <v>4.9535299999999997E-2</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.3">
@@ -1039,22 +1039,22 @@
         <v>2</v>
       </c>
       <c r="B19" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="C19">
-        <v>4.7279999999999989E-4</v>
+        <v>8.4270000000000005E-4</v>
       </c>
       <c r="D19">
-        <v>1.5681E-3</v>
+        <v>4.4114000000000002E-3</v>
       </c>
       <c r="E19">
-        <v>4.6663E-3</v>
+        <v>2.77015E-2</v>
       </c>
       <c r="F19">
-        <v>1.51979E-2</v>
+        <v>0.17886940000000001</v>
       </c>
       <c r="G19">
-        <v>5.4762749999999992E-3</v>
+        <v>5.2956250000000003E-2</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.3">
@@ -1062,22 +1062,22 @@
         <v>2</v>
       </c>
       <c r="B20" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="C20">
-        <v>5.9829999999999996E-4</v>
+        <v>9.1180000000000015E-4</v>
       </c>
       <c r="D20">
-        <v>1.7952000000000001E-3</v>
+        <v>4.4942999999999997E-3</v>
       </c>
       <c r="E20">
-        <v>6.3026999999999996E-3</v>
+        <v>2.8027300000000002E-2</v>
       </c>
       <c r="F20">
-        <v>2.30758E-2</v>
+        <v>0.17958470000000001</v>
       </c>
       <c r="G20">
-        <v>7.9430000000000004E-3</v>
+        <v>5.3254524999999997E-2</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.3">
@@ -1085,22 +1085,22 @@
         <v>2</v>
       </c>
       <c r="B21" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="C21">
-        <v>5.7279999999999994E-4</v>
+        <v>8.7040000000000001E-4</v>
       </c>
       <c r="D21">
-        <v>2.0027000000000001E-3</v>
+        <v>4.7925999999999993E-3</v>
       </c>
       <c r="E21">
-        <v>7.7119000000000007E-3</v>
+        <v>3.0382299999999991E-2</v>
       </c>
       <c r="F21">
-        <v>2.932729999999999E-2</v>
+        <v>0.1966658</v>
       </c>
       <c r="G21">
-        <v>9.9036749999999989E-3</v>
+        <v>5.8177775000000008E-2</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.3">
@@ -1108,22 +1108,22 @@
         <v>2</v>
       </c>
       <c r="B22" t="s">
-        <v>27</v>
+        <v>19</v>
       </c>
       <c r="C22">
-        <v>5.6240000000000001E-4</v>
+        <v>9.9789999999999992E-4</v>
       </c>
       <c r="D22">
-        <v>2.2937000000000001E-3</v>
+        <v>4.7220999999999999E-3</v>
       </c>
       <c r="E22">
-        <v>8.2033999999999996E-3</v>
+        <v>3.1725499999999997E-2</v>
       </c>
       <c r="F22">
-        <v>3.1877699999999988E-2</v>
+        <v>0.19733619999999999</v>
       </c>
       <c r="G22">
-        <v>1.07343E-2</v>
+        <v>5.8695425000000009E-2</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.3">
@@ -1131,22 +1131,22 @@
         <v>2</v>
       </c>
       <c r="B23" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="C23">
-        <v>8.7040000000000001E-4</v>
+        <v>1.005E-3</v>
       </c>
       <c r="D23">
-        <v>4.7925999999999993E-3</v>
+        <v>5.6778999999999996E-3</v>
       </c>
       <c r="E23">
-        <v>3.0382299999999991E-2</v>
+        <v>3.4527299999999997E-2</v>
       </c>
       <c r="F23">
-        <v>0.1966658</v>
+        <v>0.225498</v>
       </c>
       <c r="G23">
-        <v>5.8177775000000008E-2</v>
+        <v>6.6677049999999988E-2</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.3">
@@ -1154,22 +1154,22 @@
         <v>3</v>
       </c>
       <c r="B24" t="s">
-        <v>29</v>
+        <v>40</v>
       </c>
       <c r="C24">
-        <v>5.5269999999999994E-4</v>
+        <v>2.6330000000000011E-4</v>
       </c>
       <c r="D24">
-        <v>2.5788E-3</v>
+        <v>8.7900000000000012E-4</v>
       </c>
       <c r="E24">
-        <v>1.1103399999999999E-2</v>
+        <v>2.932300000000001E-3</v>
       </c>
       <c r="F24">
-        <v>5.6672599999999997E-2</v>
+        <v>1.0929700000000001E-2</v>
       </c>
       <c r="G24">
-        <v>1.7726875E-2</v>
+        <v>3.751075E-3</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.3">
@@ -1177,22 +1177,22 @@
         <v>3</v>
       </c>
       <c r="B25" t="s">
-        <v>30</v>
+        <v>39</v>
       </c>
       <c r="C25">
-        <v>5.6940000000000007E-4</v>
+        <v>4.3110000000000002E-4</v>
       </c>
       <c r="D25">
-        <v>2.4130000000000002E-3</v>
+        <v>1.3385000000000001E-3</v>
       </c>
       <c r="E25">
-        <v>1.3361E-2</v>
+        <v>4.0620000000000014E-3</v>
       </c>
       <c r="F25">
-        <v>5.5955500000000012E-2</v>
+        <v>1.4038999999999999E-2</v>
       </c>
       <c r="G25">
-        <v>1.8074725E-2</v>
+        <v>4.9676500000000014E-3</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.3">
@@ -1200,22 +1200,22 @@
         <v>3</v>
       </c>
       <c r="B26" t="s">
-        <v>31</v>
+        <v>44</v>
       </c>
       <c r="C26">
-        <v>5.7199999999999992E-4</v>
+        <v>4.6989999999999988E-4</v>
       </c>
       <c r="D26">
-        <v>2.6386999999999999E-3</v>
+        <v>1.4894999999999999E-3</v>
       </c>
       <c r="E26">
-        <v>1.2478899999999999E-2</v>
+        <v>4.9845000000000002E-3</v>
       </c>
       <c r="F26">
-        <v>6.0133600000000002E-2</v>
+        <v>1.31269E-2</v>
       </c>
       <c r="G26">
-        <v>1.8955799999999998E-2</v>
+        <v>5.0177000000000008E-3</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.3">
@@ -1223,22 +1223,22 @@
         <v>3</v>
       </c>
       <c r="B27" t="s">
-        <v>32</v>
+        <v>43</v>
       </c>
       <c r="C27">
-        <v>4.0089999999999988E-4</v>
+        <v>5.0170000000000011E-4</v>
       </c>
       <c r="D27">
-        <v>1.7438E-3</v>
+        <v>1.606E-3</v>
       </c>
       <c r="E27">
-        <v>7.4894999999999996E-3</v>
+        <v>4.5802000000000004E-3</v>
       </c>
       <c r="F27">
-        <v>3.3035500000000002E-2</v>
+        <v>1.54742E-2</v>
       </c>
       <c r="G27">
-        <v>1.0667424999999999E-2</v>
+        <v>5.5405250000000001E-3</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.3">
@@ -1246,22 +1246,22 @@
         <v>3</v>
       </c>
       <c r="B28" t="s">
-        <v>33</v>
+        <v>45</v>
       </c>
       <c r="C28">
-        <v>4.2719999999999998E-4</v>
+        <v>4.975E-4</v>
       </c>
       <c r="D28">
-        <v>1.7413999999999999E-3</v>
+        <v>1.5995E-3</v>
       </c>
       <c r="E28">
-        <v>7.4197000000000004E-3</v>
+        <v>4.5439000000000009E-3</v>
       </c>
       <c r="F28">
-        <v>3.2341699999999987E-2</v>
+        <v>1.70324E-2</v>
       </c>
       <c r="G28">
-        <v>1.04825E-2</v>
+        <v>5.9183250000000012E-3</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.3">
@@ -1269,22 +1269,22 @@
         <v>3</v>
       </c>
       <c r="B29" t="s">
-        <v>34</v>
+        <v>41</v>
       </c>
       <c r="C29">
-        <v>4.7980000000000001E-4</v>
+        <v>4.7790000000000002E-4</v>
       </c>
       <c r="D29">
-        <v>2.0875999999999998E-3</v>
+        <v>1.5106E-3</v>
       </c>
       <c r="E29">
-        <v>7.1725999999999986E-3</v>
+        <v>4.8173999999999986E-3</v>
       </c>
       <c r="F29">
-        <v>2.9955900000000001E-2</v>
+        <v>1.68845E-2</v>
       </c>
       <c r="G29">
-        <v>9.9239749999999998E-3</v>
+        <v>5.9226000000000001E-3</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.3">
@@ -1292,22 +1292,22 @@
         <v>3</v>
       </c>
       <c r="B30" t="s">
-        <v>35</v>
+        <v>42</v>
       </c>
       <c r="C30">
-        <v>1.0307999999999999E-3</v>
+        <v>3.9750000000000001E-4</v>
       </c>
       <c r="D30">
-        <v>4.8712E-3</v>
+        <v>1.2373E-3</v>
       </c>
       <c r="E30">
-        <v>3.0890299999999999E-2</v>
+        <v>4.0920000000000002E-3</v>
       </c>
       <c r="F30">
-        <v>0.19775970000000001</v>
+        <v>1.8478899999999999E-2</v>
       </c>
       <c r="G30">
-        <v>5.8638000000000003E-2</v>
+        <v>6.051425E-3</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.3">
@@ -1315,22 +1315,22 @@
         <v>3</v>
       </c>
       <c r="B31" t="s">
-        <v>36</v>
+        <v>47</v>
       </c>
       <c r="C31">
-        <v>1.0204000000000001E-3</v>
+        <v>6.0229999999999995E-4</v>
       </c>
       <c r="D31">
-        <v>5.8806000000000006E-3</v>
+        <v>1.8128E-3</v>
       </c>
       <c r="E31">
-        <v>3.4577200000000002E-2</v>
+        <v>5.8475999999999997E-3</v>
       </c>
       <c r="F31">
-        <v>0.22706989999999999</v>
+        <v>2.1591200000000001E-2</v>
       </c>
       <c r="G31">
-        <v>6.7137024999999989E-2</v>
+        <v>7.4634749999999989E-3</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.3">
@@ -1338,22 +1338,22 @@
         <v>3</v>
       </c>
       <c r="B32" t="s">
-        <v>37</v>
+        <v>46</v>
       </c>
       <c r="C32">
-        <v>1.0491000000000001E-3</v>
+        <v>6.198E-4</v>
       </c>
       <c r="D32">
-        <v>5.8165999999999999E-3</v>
+        <v>1.8263000000000001E-3</v>
       </c>
       <c r="E32">
-        <v>3.3596599999999997E-2</v>
+        <v>6.4658000000000007E-3</v>
       </c>
       <c r="F32">
-        <v>0.22013679999999999</v>
+        <v>2.3189999999999999E-2</v>
       </c>
       <c r="G32">
-        <v>6.5149774999999993E-2</v>
+        <v>8.0254750000000007E-3</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.3">
@@ -1361,22 +1361,22 @@
         <v>3</v>
       </c>
       <c r="B33" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="C33">
-        <v>8.7679999999999995E-4</v>
+        <v>4.7980000000000001E-4</v>
       </c>
       <c r="D33">
-        <v>4.5497999999999997E-3</v>
+        <v>2.0875999999999998E-3</v>
       </c>
       <c r="E33">
-        <v>2.6851400000000001E-2</v>
+        <v>7.1725999999999986E-3</v>
       </c>
       <c r="F33">
-        <v>0.167374</v>
+        <v>2.9955900000000001E-2</v>
       </c>
       <c r="G33">
-        <v>4.9912999999999999E-2</v>
+        <v>9.9239749999999998E-3</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.3">
@@ -1384,22 +1384,22 @@
         <v>3</v>
       </c>
       <c r="B34" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="C34">
-        <v>4.3110000000000002E-4</v>
+        <v>4.2719999999999998E-4</v>
       </c>
       <c r="D34">
-        <v>1.3385000000000001E-3</v>
+        <v>1.7413999999999999E-3</v>
       </c>
       <c r="E34">
-        <v>4.0620000000000014E-3</v>
+        <v>7.4197000000000004E-3</v>
       </c>
       <c r="F34">
-        <v>1.4038999999999999E-2</v>
+        <v>3.2341699999999987E-2</v>
       </c>
       <c r="G34">
-        <v>4.9676500000000014E-3</v>
+        <v>1.04825E-2</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.3">
@@ -1407,22 +1407,22 @@
         <v>3</v>
       </c>
       <c r="B35" t="s">
-        <v>40</v>
+        <v>32</v>
       </c>
       <c r="C35">
-        <v>2.6330000000000011E-4</v>
+        <v>4.0089999999999988E-4</v>
       </c>
       <c r="D35">
-        <v>8.7900000000000012E-4</v>
+        <v>1.7438E-3</v>
       </c>
       <c r="E35">
-        <v>2.932300000000001E-3</v>
+        <v>7.4894999999999996E-3</v>
       </c>
       <c r="F35">
-        <v>1.0929700000000001E-2</v>
+        <v>3.3035500000000002E-2</v>
       </c>
       <c r="G35">
-        <v>3.751075E-3</v>
+        <v>1.0667424999999999E-2</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.3">
@@ -1430,22 +1430,22 @@
         <v>3</v>
       </c>
       <c r="B36" t="s">
-        <v>41</v>
+        <v>48</v>
       </c>
       <c r="C36">
-        <v>4.7790000000000002E-4</v>
+        <v>5.8700000000000007E-4</v>
       </c>
       <c r="D36">
-        <v>1.5106E-3</v>
+        <v>2.2431999999999999E-3</v>
       </c>
       <c r="E36">
-        <v>4.8173999999999986E-3</v>
+        <v>8.3339E-3</v>
       </c>
       <c r="F36">
-        <v>1.68845E-2</v>
+        <v>3.3125099999999998E-2</v>
       </c>
       <c r="G36">
-        <v>5.9226000000000001E-3</v>
+        <v>1.10723E-2</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.3">
@@ -1453,22 +1453,22 @@
         <v>3</v>
       </c>
       <c r="B37" t="s">
-        <v>42</v>
+        <v>29</v>
       </c>
       <c r="C37">
-        <v>3.9750000000000001E-4</v>
+        <v>5.5269999999999994E-4</v>
       </c>
       <c r="D37">
-        <v>1.2373E-3</v>
+        <v>2.5788E-3</v>
       </c>
       <c r="E37">
-        <v>4.0920000000000002E-3</v>
+        <v>1.1103399999999999E-2</v>
       </c>
       <c r="F37">
-        <v>1.8478899999999999E-2</v>
+        <v>5.6672599999999997E-2</v>
       </c>
       <c r="G37">
-        <v>6.051425E-3</v>
+        <v>1.7726875E-2</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.3">
@@ -1476,22 +1476,22 @@
         <v>3</v>
       </c>
       <c r="B38" t="s">
-        <v>43</v>
+        <v>30</v>
       </c>
       <c r="C38">
-        <v>5.0170000000000011E-4</v>
+        <v>5.6940000000000007E-4</v>
       </c>
       <c r="D38">
-        <v>1.606E-3</v>
+        <v>2.4130000000000002E-3</v>
       </c>
       <c r="E38">
-        <v>4.5802000000000004E-3</v>
+        <v>1.3361E-2</v>
       </c>
       <c r="F38">
-        <v>1.54742E-2</v>
+        <v>5.5955500000000012E-2</v>
       </c>
       <c r="G38">
-        <v>5.5405250000000001E-3</v>
+        <v>1.8074725E-2</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.3">
@@ -1499,22 +1499,22 @@
         <v>3</v>
       </c>
       <c r="B39" t="s">
-        <v>44</v>
+        <v>31</v>
       </c>
       <c r="C39">
-        <v>4.6989999999999988E-4</v>
+        <v>5.7199999999999992E-4</v>
       </c>
       <c r="D39">
-        <v>1.4894999999999999E-3</v>
+        <v>2.6386999999999999E-3</v>
       </c>
       <c r="E39">
-        <v>4.9845000000000002E-3</v>
+        <v>1.2478899999999999E-2</v>
       </c>
       <c r="F39">
-        <v>1.31269E-2</v>
+        <v>6.0133600000000002E-2</v>
       </c>
       <c r="G39">
-        <v>5.0177000000000008E-3</v>
+        <v>1.8955799999999998E-2</v>
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.3">
@@ -1522,22 +1522,22 @@
         <v>3</v>
       </c>
       <c r="B40" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="C40">
-        <v>4.975E-4</v>
+        <v>8.7679999999999995E-4</v>
       </c>
       <c r="D40">
-        <v>1.5995E-3</v>
+        <v>4.5497999999999997E-3</v>
       </c>
       <c r="E40">
-        <v>4.5439000000000009E-3</v>
+        <v>2.6851400000000001E-2</v>
       </c>
       <c r="F40">
-        <v>1.70324E-2</v>
+        <v>0.167374</v>
       </c>
       <c r="G40">
-        <v>5.9183250000000012E-3</v>
+        <v>4.9912999999999999E-2</v>
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.3">
@@ -1545,22 +1545,22 @@
         <v>3</v>
       </c>
       <c r="B41" t="s">
-        <v>46</v>
+        <v>35</v>
       </c>
       <c r="C41">
-        <v>6.198E-4</v>
+        <v>1.0307999999999999E-3</v>
       </c>
       <c r="D41">
-        <v>1.8263000000000001E-3</v>
+        <v>4.8712E-3</v>
       </c>
       <c r="E41">
-        <v>6.4658000000000007E-3</v>
+        <v>3.0890299999999999E-2</v>
       </c>
       <c r="F41">
-        <v>2.3189999999999999E-2</v>
+        <v>0.19775970000000001</v>
       </c>
       <c r="G41">
-        <v>8.0254750000000007E-3</v>
+        <v>5.8638000000000003E-2</v>
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.3">
@@ -1568,22 +1568,22 @@
         <v>3</v>
       </c>
       <c r="B42" t="s">
-        <v>47</v>
+        <v>37</v>
       </c>
       <c r="C42">
-        <v>6.0229999999999995E-4</v>
+        <v>1.0491000000000001E-3</v>
       </c>
       <c r="D42">
-        <v>1.8128E-3</v>
+        <v>5.8165999999999999E-3</v>
       </c>
       <c r="E42">
-        <v>5.8475999999999997E-3</v>
+        <v>3.3596599999999997E-2</v>
       </c>
       <c r="F42">
-        <v>2.1591200000000001E-2</v>
+        <v>0.22013679999999999</v>
       </c>
       <c r="G42">
-        <v>7.4634749999999989E-3</v>
+        <v>6.5149774999999993E-2</v>
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.3">
@@ -1591,22 +1591,22 @@
         <v>3</v>
       </c>
       <c r="B43" t="s">
-        <v>48</v>
+        <v>36</v>
       </c>
       <c r="C43">
-        <v>5.8700000000000007E-4</v>
+        <v>1.0204000000000001E-3</v>
       </c>
       <c r="D43">
-        <v>2.2431999999999999E-3</v>
+        <v>5.8806000000000006E-3</v>
       </c>
       <c r="E43">
-        <v>8.3339E-3</v>
+        <v>3.4577200000000002E-2</v>
       </c>
       <c r="F43">
-        <v>3.3125099999999998E-2</v>
+        <v>0.22706989999999999</v>
       </c>
       <c r="G43">
-        <v>1.10723E-2</v>
+        <v>6.7137024999999989E-2</v>
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.3">
@@ -1614,22 +1614,22 @@
         <v>4</v>
       </c>
       <c r="B44" t="s">
-        <v>49</v>
+        <v>56</v>
       </c>
       <c r="C44">
-        <v>6.3170000000000001E-4</v>
+        <v>3.3599999999999998E-4</v>
       </c>
       <c r="D44">
-        <v>2.6078E-3</v>
+        <v>9.6270000000000004E-4</v>
       </c>
       <c r="E44">
-        <v>1.24546E-2</v>
+        <v>2.9889999999999999E-3</v>
       </c>
       <c r="F44">
-        <v>5.67871E-2</v>
+        <v>1.1006200000000001E-2</v>
       </c>
       <c r="G44">
-        <v>1.8120299999999999E-2</v>
+        <v>3.8234749999999998E-3</v>
       </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.3">
@@ -1637,22 +1637,22 @@
         <v>4</v>
       </c>
       <c r="B45" t="s">
-        <v>50</v>
+        <v>57</v>
       </c>
       <c r="C45">
-        <v>5.8759999999999997E-4</v>
+        <v>3.1470000000000001E-4</v>
       </c>
       <c r="D45">
-        <v>2.8303E-3</v>
+        <v>1.0001999999999999E-3</v>
       </c>
       <c r="E45">
-        <v>1.22928E-2</v>
+        <v>3.0230999999999999E-3</v>
       </c>
       <c r="F45">
-        <v>6.0997100000000012E-2</v>
+        <v>1.1051200000000001E-2</v>
       </c>
       <c r="G45">
-        <v>1.9176950000000002E-2</v>
+        <v>3.8473000000000001E-3</v>
       </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.3">
@@ -1660,22 +1660,22 @@
         <v>4</v>
       </c>
       <c r="B46" t="s">
-        <v>51</v>
+        <v>60</v>
       </c>
       <c r="C46">
-        <v>5.7959999999999989E-4</v>
+        <v>5.2250000000000007E-4</v>
       </c>
       <c r="D46">
-        <v>2.7095999999999999E-3</v>
+        <v>1.5704E-3</v>
       </c>
       <c r="E46">
-        <v>1.1530200000000001E-2</v>
+        <v>3.9540999999999986E-3</v>
       </c>
       <c r="F46">
-        <v>5.7557099999999993E-2</v>
+        <v>1.35342E-2</v>
       </c>
       <c r="G46">
-        <v>1.8094124999999999E-2</v>
+        <v>4.8953E-3</v>
       </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.3">
@@ -1683,22 +1683,22 @@
         <v>4</v>
       </c>
       <c r="B47" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="C47">
-        <v>4.5679999999999999E-4</v>
+        <v>4.8069999999999997E-4</v>
       </c>
       <c r="D47">
-        <v>1.9105000000000001E-3</v>
+        <v>1.3879999999999999E-3</v>
       </c>
       <c r="E47">
-        <v>7.7654999999999998E-3</v>
+        <v>4.1368000000000004E-3</v>
       </c>
       <c r="F47">
-        <v>3.3472600000000012E-2</v>
+        <v>1.4173099999999999E-2</v>
       </c>
       <c r="G47">
-        <v>1.0901350000000001E-2</v>
+        <v>5.0446499999999986E-3</v>
       </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.3">
@@ -1706,22 +1706,22 @@
         <v>4</v>
       </c>
       <c r="B48" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="C48">
-        <v>1.1359E-3</v>
+        <v>4.4200000000000001E-4</v>
       </c>
       <c r="D48">
-        <v>6.0593000000000001E-3</v>
+        <v>1.3045999999999999E-3</v>
       </c>
       <c r="E48">
-        <v>3.4112900000000002E-2</v>
+        <v>3.9623000000000002E-3</v>
       </c>
       <c r="F48">
-        <v>0.2212797</v>
+        <v>1.54468E-2</v>
       </c>
       <c r="G48">
-        <v>6.5646950000000009E-2</v>
+        <v>5.2889249999999999E-3</v>
       </c>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.3">
@@ -1729,22 +1729,22 @@
         <v>4</v>
       </c>
       <c r="B49" t="s">
-        <v>54</v>
+        <v>62</v>
       </c>
       <c r="C49">
-        <v>4.8069999999999997E-4</v>
+        <v>5.1840000000000002E-4</v>
       </c>
       <c r="D49">
-        <v>1.3879999999999999E-3</v>
+        <v>1.6442E-3</v>
       </c>
       <c r="E49">
-        <v>4.1368000000000004E-3</v>
+        <v>4.5433000000000001E-3</v>
       </c>
       <c r="F49">
-        <v>1.4173099999999999E-2</v>
+        <v>1.68763E-2</v>
       </c>
       <c r="G49">
-        <v>5.0446499999999986E-3</v>
+        <v>5.8955500000000011E-3</v>
       </c>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.3">
@@ -1752,22 +1752,22 @@
         <v>4</v>
       </c>
       <c r="B50" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="C50">
-        <v>4.4200000000000001E-4</v>
+        <v>5.6980000000000008E-4</v>
       </c>
       <c r="D50">
-        <v>1.3045999999999999E-3</v>
+        <v>1.6581E-3</v>
       </c>
       <c r="E50">
-        <v>3.9623000000000002E-3</v>
+        <v>4.6348000000000014E-3</v>
       </c>
       <c r="F50">
-        <v>1.54468E-2</v>
+        <v>1.7063499999999999E-2</v>
       </c>
       <c r="G50">
-        <v>5.2889249999999999E-3</v>
+        <v>5.9815500000000004E-3</v>
       </c>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.3">
@@ -1775,22 +1775,22 @@
         <v>4</v>
       </c>
       <c r="B51" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="C51">
-        <v>3.3599999999999998E-4</v>
+        <v>2.9250000000000001E-4</v>
       </c>
       <c r="D51">
-        <v>9.6270000000000004E-4</v>
+        <v>9.6199999999999996E-4</v>
       </c>
       <c r="E51">
-        <v>2.9889999999999999E-3</v>
+        <v>3.9028000000000001E-3</v>
       </c>
       <c r="F51">
-        <v>1.1006200000000001E-2</v>
+        <v>1.89211E-2</v>
       </c>
       <c r="G51">
-        <v>3.8234749999999998E-3</v>
+        <v>6.0196000000000008E-3</v>
       </c>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.3">
@@ -1798,22 +1798,22 @@
         <v>4</v>
       </c>
       <c r="B52" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="C52">
-        <v>3.1470000000000001E-4</v>
+        <v>4.3370000000000003E-4</v>
       </c>
       <c r="D52">
-        <v>1.0001999999999999E-3</v>
+        <v>1.2313000000000001E-3</v>
       </c>
       <c r="E52">
-        <v>3.0230999999999999E-3</v>
+        <v>4.1329000000000001E-3</v>
       </c>
       <c r="F52">
-        <v>1.1051200000000001E-2</v>
+        <v>1.9089800000000001E-2</v>
       </c>
       <c r="G52">
-        <v>3.8473000000000001E-3</v>
+        <v>6.2219249999999997E-3</v>
       </c>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.3">
@@ -1821,22 +1821,22 @@
         <v>4</v>
       </c>
       <c r="B53" t="s">
-        <v>58</v>
+        <v>63</v>
       </c>
       <c r="C53">
-        <v>2.9250000000000001E-4</v>
+        <v>6.3679999999999997E-4</v>
       </c>
       <c r="D53">
-        <v>9.6199999999999996E-4</v>
+        <v>1.8515999999999999E-3</v>
       </c>
       <c r="E53">
-        <v>3.9028000000000001E-3</v>
+        <v>5.7964999999999996E-3</v>
       </c>
       <c r="F53">
-        <v>1.89211E-2</v>
+        <v>2.20091E-2</v>
       </c>
       <c r="G53">
-        <v>6.0196000000000008E-3</v>
+        <v>7.5735000000000004E-3</v>
       </c>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.3">
@@ -1844,22 +1844,22 @@
         <v>4</v>
       </c>
       <c r="B54" t="s">
-        <v>59</v>
+        <v>52</v>
       </c>
       <c r="C54">
-        <v>4.3370000000000003E-4</v>
+        <v>4.5679999999999999E-4</v>
       </c>
       <c r="D54">
-        <v>1.2313000000000001E-3</v>
+        <v>1.9105000000000001E-3</v>
       </c>
       <c r="E54">
-        <v>4.1329000000000001E-3</v>
+        <v>7.7654999999999998E-3</v>
       </c>
       <c r="F54">
-        <v>1.9089800000000001E-2</v>
+        <v>3.3472600000000012E-2</v>
       </c>
       <c r="G54">
-        <v>6.2219249999999997E-3</v>
+        <v>1.0901350000000001E-2</v>
       </c>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.3">
@@ -1867,22 +1867,22 @@
         <v>4</v>
       </c>
       <c r="B55" t="s">
-        <v>60</v>
+        <v>51</v>
       </c>
       <c r="C55">
-        <v>5.2250000000000007E-4</v>
+        <v>5.7959999999999989E-4</v>
       </c>
       <c r="D55">
-        <v>1.5704E-3</v>
+        <v>2.7095999999999999E-3</v>
       </c>
       <c r="E55">
-        <v>3.9540999999999986E-3</v>
+        <v>1.1530200000000001E-2</v>
       </c>
       <c r="F55">
-        <v>1.35342E-2</v>
+        <v>5.7557099999999993E-2</v>
       </c>
       <c r="G55">
-        <v>4.8953E-3</v>
+        <v>1.8094124999999999E-2</v>
       </c>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.3">
@@ -1890,22 +1890,22 @@
         <v>4</v>
       </c>
       <c r="B56" t="s">
-        <v>61</v>
+        <v>49</v>
       </c>
       <c r="C56">
-        <v>5.6980000000000008E-4</v>
+        <v>6.3170000000000001E-4</v>
       </c>
       <c r="D56">
-        <v>1.6581E-3</v>
+        <v>2.6078E-3</v>
       </c>
       <c r="E56">
-        <v>4.6348000000000014E-3</v>
+        <v>1.24546E-2</v>
       </c>
       <c r="F56">
-        <v>1.7063499999999999E-2</v>
+        <v>5.67871E-2</v>
       </c>
       <c r="G56">
-        <v>5.9815500000000004E-3</v>
+        <v>1.8120299999999999E-2</v>
       </c>
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.3">
@@ -1913,22 +1913,22 @@
         <v>4</v>
       </c>
       <c r="B57" t="s">
-        <v>62</v>
+        <v>50</v>
       </c>
       <c r="C57">
-        <v>5.1840000000000002E-4</v>
+        <v>5.8759999999999997E-4</v>
       </c>
       <c r="D57">
-        <v>1.6442E-3</v>
+        <v>2.8303E-3</v>
       </c>
       <c r="E57">
-        <v>4.5433000000000001E-3</v>
+        <v>1.22928E-2</v>
       </c>
       <c r="F57">
-        <v>1.68763E-2</v>
+        <v>6.0997100000000012E-2</v>
       </c>
       <c r="G57">
-        <v>5.8955500000000011E-3</v>
+        <v>1.9176950000000002E-2</v>
       </c>
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.3">
@@ -1936,22 +1936,22 @@
         <v>4</v>
       </c>
       <c r="B58" t="s">
-        <v>63</v>
+        <v>53</v>
       </c>
       <c r="C58">
-        <v>6.3679999999999997E-4</v>
+        <v>1.1359E-3</v>
       </c>
       <c r="D58">
-        <v>1.8515999999999999E-3</v>
+        <v>6.0593000000000001E-3</v>
       </c>
       <c r="E58">
-        <v>5.7964999999999996E-3</v>
+        <v>3.4112900000000002E-2</v>
       </c>
       <c r="F58">
-        <v>2.20091E-2</v>
+        <v>0.2212797</v>
       </c>
       <c r="G58">
-        <v>7.5735000000000004E-3</v>
+        <v>6.5646950000000009E-2</v>
       </c>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.3">
@@ -1959,22 +1959,22 @@
         <v>5</v>
       </c>
       <c r="B59" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="C59">
-        <v>6.4560000000000008E-4</v>
+        <v>3.8249999999999997E-4</v>
       </c>
       <c r="D59">
-        <v>2.8408000000000001E-3</v>
+        <v>1.0116999999999999E-3</v>
       </c>
       <c r="E59">
-        <v>1.2025599999999999E-2</v>
+        <v>3.2128E-3</v>
       </c>
       <c r="F59">
-        <v>5.8474999999999999E-2</v>
+        <v>1.11264E-2</v>
       </c>
       <c r="G59">
-        <v>1.8496749999999999E-2</v>
+        <v>3.9333500000000004E-3</v>
       </c>
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.3">
@@ -2005,22 +2005,22 @@
         <v>5</v>
       </c>
       <c r="B61" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="C61">
-        <v>3.8249999999999997E-4</v>
+        <v>3.6549999999999999E-4</v>
       </c>
       <c r="D61">
-        <v>1.0116999999999999E-3</v>
+        <v>1.0134E-3</v>
       </c>
       <c r="E61">
-        <v>3.2128E-3</v>
+        <v>3.6587E-3</v>
       </c>
       <c r="F61">
-        <v>1.11264E-2</v>
+        <v>1.7533699999999999E-2</v>
       </c>
       <c r="G61">
-        <v>3.9333500000000004E-3</v>
+        <v>5.6428249999999998E-3</v>
       </c>
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.3">
@@ -2028,22 +2028,22 @@
         <v>5</v>
       </c>
       <c r="B62" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="C62">
-        <v>3.6549999999999999E-4</v>
+        <v>5.6540000000000008E-4</v>
       </c>
       <c r="D62">
-        <v>1.0134E-3</v>
+        <v>1.6704999999999999E-3</v>
       </c>
       <c r="E62">
-        <v>3.6587E-3</v>
+        <v>4.7204000000000013E-3</v>
       </c>
       <c r="F62">
-        <v>1.7533699999999999E-2</v>
+        <v>1.7070599999999998E-2</v>
       </c>
       <c r="G62">
-        <v>5.6428249999999998E-3</v>
+        <v>6.006725000000001E-3</v>
       </c>
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.3">
@@ -2074,22 +2074,22 @@
         <v>5</v>
       </c>
       <c r="B64" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="C64">
-        <v>5.6540000000000008E-4</v>
+        <v>6.4560000000000008E-4</v>
       </c>
       <c r="D64">
-        <v>1.6704999999999999E-3</v>
+        <v>2.8408000000000001E-3</v>
       </c>
       <c r="E64">
-        <v>4.7204000000000013E-3</v>
+        <v>1.2025599999999999E-2</v>
       </c>
       <c r="F64">
-        <v>1.7070599999999998E-2</v>
+        <v>5.8474999999999999E-2</v>
       </c>
       <c r="G64">
-        <v>6.006725000000001E-3</v>
+        <v>1.8496749999999999E-2</v>
       </c>
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.3">
@@ -2118,8 +2118,7 @@
   </sheetData>
   <autoFilter ref="A1:G65" xr:uid="{00000000-0001-0000-0000-000000000000}">
     <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G65">
-      <sortCondition ref="A2:A65"/>
-      <sortCondition ref="B2:B65"/>
+      <sortCondition ref="A1:A65"/>
     </sortState>
   </autoFilter>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G7">

</xml_diff>